<commit_message>
RDM-7072: Latest from 6155
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/aat/resources/CCD_BEFTA_JURISDICTION2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sivakanukollu/github/MOJ/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/475495/Documents/Home/Development/06-Jan/ccd-data-store/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B71DE8-E636-1640-8018-5733A0B89AC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0C49FD-B3B7-E942-8039-1E4CE10985C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12900" yWindow="-21320" windowWidth="28800" windowHeight="16480" tabRatio="823" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -5047,8 +5047,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="F126" sqref="F126"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119:D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7113,7 +7113,7 @@
         <v>267</v>
       </c>
       <c r="F119" s="24" t="s">
-        <v>292</v>
+        <v>123</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7131,7 +7131,7 @@
         <v>267</v>
       </c>
       <c r="F120" s="24" t="s">
-        <v>123</v>
+        <v>296</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7149,7 +7149,7 @@
         <v>267</v>
       </c>
       <c r="F121" s="24" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7185,7 +7185,7 @@
         <v>267</v>
       </c>
       <c r="F123" s="24" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7203,7 +7203,7 @@
         <v>267</v>
       </c>
       <c r="F124" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7221,7 +7221,7 @@
         <v>267</v>
       </c>
       <c r="F125" s="24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7282,7 +7282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="144" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="144" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>